<commit_message>
Tests added: - Download one under limit - Download above limit - Download time limit - Download after time limit (not finished) - Upload file above MB limit (not finished)
</commit_message>
<xml_diff>
--- a/Test Cases.xlsx
+++ b/Test Cases.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SELENIUM NAUKA\TMP_Files_Testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SELENIUM NAUKA\TMP_Files_Testing_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BA4F60D-C016-4331-ADBB-08D5D1BDCF6A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52518AE6-86F8-4C29-967F-7D776C96AB7A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{D93F8B92-B182-4C84-9291-ECED4203DC4B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
   <si>
     <t>1.</t>
   </si>
@@ -139,16 +139,39 @@
   </si>
   <si>
     <t>Already uploaded file and ready to use link to it.</t>
+  </si>
+  <si>
+    <t>10.</t>
+  </si>
+  <si>
+    <t>Expect to have errors about wrong data in limit fields.</t>
+  </si>
+  <si>
+    <t>Upload fields random data check w/ file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11. </t>
+  </si>
+  <si>
+    <t>Upload fields random data check w/o file</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
@@ -175,8 +198,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -491,15 +515,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F9CA6EF-F820-4DA2-BAC8-6A648B2E0378}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="33.28515625" customWidth="1"/>
+    <col min="2" max="2" width="39.5703125" customWidth="1"/>
     <col min="3" max="3" width="114.5703125" customWidth="1"/>
     <col min="4" max="4" width="79.42578125" customWidth="1"/>
   </cols>
@@ -522,7 +546,7 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C2" t="s">
@@ -536,7 +560,7 @@
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C3" t="s">
@@ -550,7 +574,7 @@
       <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C4" t="s">
@@ -564,7 +588,7 @@
       <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C5" t="s">
@@ -578,7 +602,7 @@
       <c r="A6" t="s">
         <v>15</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C6" t="s">
@@ -592,7 +616,7 @@
       <c r="A7" t="s">
         <v>18</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C7" t="s">
@@ -644,7 +668,27 @@
         <v>37</v>
       </c>
     </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>